<commit_message>
Adding new notebook for transfection efficiency and cell viability comparison
</commit_message>
<xml_diff>
--- a/PicoGreen_Plots/20240119_PicoGreen_DIPLibrary_Water-PBS.xlsx
+++ b/PicoGreen_Plots/20240119_PicoGreen_DIPLibrary_Water-PBS.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Documents - Aryelle’s MacBook Air/Kumar-Biomaterials-Lab/PicoGreen_Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B944994B-7BA9-C543-AD68-D5EBA1845112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F687F81-ADAF-434D-AA95-46B5E521EA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="660" windowWidth="19180" windowHeight="13100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="1380" windowWidth="23860" windowHeight="16120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="water" sheetId="2" r:id="rId2"/>
-    <sheet name="water-python" sheetId="4" r:id="rId3"/>
-    <sheet name="PBS" sheetId="3" r:id="rId4"/>
-    <sheet name="pbs-python" sheetId="5" r:id="rId5"/>
+    <sheet name="p-test_water" sheetId="6" r:id="rId2"/>
+    <sheet name="water" sheetId="2" r:id="rId3"/>
+    <sheet name="water-python" sheetId="4" r:id="rId4"/>
+    <sheet name="PBS" sheetId="3" r:id="rId5"/>
+    <sheet name="pbs-python" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="MethodPointer1">-10455696</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="73">
   <si>
     <t>Software Version</t>
   </si>
@@ -260,6 +261,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G3 </t>
   </si>
 </sst>
 </file>
@@ -392,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -436,6 +440,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:O45"/>
+  <dimension ref="A2:V53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1316,6 +1321,135 @@
         <v>6</v>
       </c>
     </row>
+    <row r="51" spans="2:22" x14ac:dyDescent="0.15">
+      <c r="B51" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H51" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I51" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J51" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K51" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L51" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M51" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="N51" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="O51" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="P51" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q51" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="R51" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="S51" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="T51" s="16"/>
+      <c r="U51" s="16"/>
+      <c r="V51" s="16"/>
+    </row>
+    <row r="52" spans="2:22" x14ac:dyDescent="0.15">
+      <c r="B52" s="10">
+        <v>9776</v>
+      </c>
+      <c r="C52" s="10">
+        <v>9882</v>
+      </c>
+      <c r="D52" s="10">
+        <v>9483</v>
+      </c>
+      <c r="E52" s="9">
+        <v>873</v>
+      </c>
+      <c r="F52" s="9">
+        <v>909</v>
+      </c>
+      <c r="G52" s="9">
+        <v>925</v>
+      </c>
+      <c r="H52" s="9">
+        <v>103</v>
+      </c>
+      <c r="I52" s="9">
+        <v>139</v>
+      </c>
+      <c r="J52" s="9">
+        <v>111</v>
+      </c>
+      <c r="K52" s="9">
+        <v>659</v>
+      </c>
+      <c r="L52" s="9">
+        <v>599</v>
+      </c>
+      <c r="M52" s="9">
+        <v>540</v>
+      </c>
+      <c r="N52" s="9">
+        <v>477</v>
+      </c>
+      <c r="O52" s="9">
+        <v>469</v>
+      </c>
+      <c r="P52" s="9">
+        <v>518</v>
+      </c>
+      <c r="Q52" s="9">
+        <v>833</v>
+      </c>
+      <c r="R52" s="9">
+        <v>835</v>
+      </c>
+      <c r="S52" s="9">
+        <v>822</v>
+      </c>
+      <c r="T52" s="10"/>
+      <c r="U52" s="10"/>
+      <c r="V52" s="10"/>
+    </row>
+    <row r="53" spans="2:22" x14ac:dyDescent="0.15">
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1325,11 +1459,228 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D221602-1A9B-574D-98A8-35822E79A344}">
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="10">
+        <v>9776</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A2" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="10">
+        <v>9882</v>
+      </c>
+      <c r="C2" s="10">
+        <v>9483</v>
+      </c>
+      <c r="D2" s="9">
+        <v>873</v>
+      </c>
+      <c r="E2" s="9">
+        <v>909</v>
+      </c>
+      <c r="F2" s="9">
+        <v>925</v>
+      </c>
+      <c r="G2" s="9">
+        <v>103</v>
+      </c>
+      <c r="H2" s="9">
+        <v>139</v>
+      </c>
+      <c r="I2" s="9">
+        <v>111</v>
+      </c>
+      <c r="J2" s="9">
+        <v>659</v>
+      </c>
+      <c r="K2" s="9">
+        <v>599</v>
+      </c>
+      <c r="L2" s="9">
+        <v>540</v>
+      </c>
+      <c r="M2" s="9">
+        <v>477</v>
+      </c>
+      <c r="N2" s="9">
+        <v>469</v>
+      </c>
+      <c r="O2" s="9">
+        <v>518</v>
+      </c>
+      <c r="P2" s="9">
+        <v>833</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>835</v>
+      </c>
+      <c r="R2" s="9">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A3" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="10">
+        <v>9483</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A4" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="9">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A5" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="9">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A6" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="9">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="9">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A8" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A9" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A10" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A11" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A12" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A13" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A14" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A15" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A16" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C810B7EF-F5AF-A34B-B39C-94421765E95E}">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:I20"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1578,12 +1929,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1DFC87-FB17-6B41-8DD9-1518A6F51664}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1670,7 +2021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1973EB3C-F83B-CB49-90D5-C093FE611B6A}">
   <dimension ref="A1:I19"/>
   <sheetViews>
@@ -1916,7 +2267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFC3693A-F1BA-444B-9778-3B2CB00A395C}">
   <dimension ref="A1:C7"/>
   <sheetViews>

</xml_diff>